<commit_message>
statuses methods and storage created
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MunchkinML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B1F16D-F11D-4D67-960B-378019A95FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222151C8-9BE4-4C52-AA40-625A899746D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756F23DA-8B2B-43D1-941C-E221060CE055}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{756F23DA-8B2B-43D1-941C-E221060CE055}"/>
   </bookViews>
   <sheets>
     <sheet name="monsters" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="791">
   <si>
     <t>were_turtle</t>
   </si>
@@ -2248,9 +2248,6 @@
     <t>never</t>
   </si>
   <si>
-    <t>agains all grasses -10</t>
-  </si>
-  <si>
     <t>self.player.add_status('fight_level_only')</t>
   </si>
   <si>
@@ -2389,9 +2386,6 @@
     <t>self.monster.update_level(+5) if 'halfling'  in self.player.race else ''</t>
   </si>
   <si>
-    <t>self.monster.update_level(+5) if 'orc' in self.player.race else '';self.monster.update_level(+5) if 'warrior'  in self.player.plcass else ''</t>
-  </si>
-  <si>
     <t>self.monster.update_level(+3) if len(self.player.pclass)==0 else ''</t>
   </si>
   <si>
@@ -2438,6 +2432,15 @@
   </si>
   <si>
     <t>self.player.update_pclass_race('race', n=-1, make_decision=True)</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>self.monster.update_level(+5) if 'orc' in self.player.race else '';self.monster.update_level(+5) if 'warrior' in self.player.pclass else ''</t>
+  </si>
+  <si>
+    <t>self.monster.update_level(+10) if self.monster.name in GLOBAL_MONSTER_GRASS else ''</t>
   </si>
 </sst>
 </file>
@@ -2926,8 +2929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{835D834E-D9E6-49F6-98E3-A07AA920BC51}">
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2990,10 +2993,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -3022,10 +3025,10 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -3054,16 +3057,16 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -3086,10 +3089,10 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -3118,10 +3121,10 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -3150,10 +3153,10 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -3182,10 +3185,10 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -3214,16 +3217,16 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -3246,16 +3249,16 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -3278,10 +3281,10 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -3310,10 +3313,10 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -3342,10 +3345,10 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -3374,10 +3377,10 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -3409,7 +3412,7 @@
         <v>52</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -3441,7 +3444,7 @@
         <v>720</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
@@ -3473,7 +3476,7 @@
         <v>51</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -3502,10 +3505,10 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -3534,10 +3537,10 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
@@ -3566,16 +3569,16 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="I20">
         <v>1</v>
@@ -3598,16 +3601,16 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G21" t="b">
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -3630,10 +3633,10 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G22" t="b">
         <v>1</v>
@@ -3662,10 +3665,10 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G23" t="b">
         <v>1</v>
@@ -3694,10 +3697,10 @@
         <v>0</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G24" s="2" t="b">
         <v>1</v>
@@ -3726,16 +3729,16 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="F25" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G25" t="b">
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="I25">
         <v>2</v>
@@ -3761,7 +3764,7 @@
         <v>51</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G26" t="b">
         <v>1</v>
@@ -3790,10 +3793,10 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G27" t="b">
         <v>1</v>
@@ -3822,10 +3825,10 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G28" t="b">
         <v>1</v>
@@ -3854,10 +3857,10 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G29" t="b">
         <v>1</v>
@@ -3886,10 +3889,10 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G30" t="b">
         <v>1</v>
@@ -3918,10 +3921,10 @@
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G31" t="b">
         <v>1</v>
@@ -3950,7 +3953,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F32" t="s">
         <v>493</v>
@@ -3982,10 +3985,10 @@
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G33" t="b">
         <v>1</v>
@@ -4014,10 +4017,10 @@
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G34" t="b">
         <v>1</v>
@@ -4046,10 +4049,10 @@
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G35" t="b">
         <v>1</v>
@@ -4078,16 +4081,16 @@
         <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G36" t="b">
         <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="I36">
         <v>1</v>
@@ -4110,10 +4113,10 @@
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G37" t="b">
         <v>1</v>
@@ -4142,10 +4145,10 @@
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G38" t="b">
         <v>1</v>
@@ -4174,16 +4177,16 @@
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G39" t="b">
         <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="I39">
         <v>1</v>
@@ -4206,10 +4209,10 @@
         <v>0</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G40" t="b">
         <v>1</v>
@@ -4238,10 +4241,10 @@
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G41" t="b">
         <v>1</v>
@@ -4273,7 +4276,7 @@
         <v>46</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G42" t="b">
         <v>1</v>
@@ -4301,17 +4304,17 @@
       <c r="D43" t="b">
         <v>0</v>
       </c>
-      <c r="E43" t="s">
-        <v>773</v>
+      <c r="E43" s="14" t="s">
+        <v>789</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G43" t="b">
         <v>1</v>
       </c>
       <c r="H43" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="I43">
         <v>1</v>
@@ -4334,10 +4337,10 @@
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G44" t="b">
         <v>1</v>
@@ -4366,16 +4369,16 @@
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G45" t="b">
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="I45">
         <v>1</v>
@@ -4398,10 +4401,10 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G46" t="b">
         <v>1</v>
@@ -4430,10 +4433,10 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G47" t="b">
         <v>1</v>
@@ -4462,10 +4465,10 @@
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G48" t="b">
         <v>1</v>
@@ -4497,13 +4500,13 @@
         <v>40</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G49" t="b">
         <v>1</v>
       </c>
       <c r="H49" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="I49">
         <v>1</v>
@@ -4526,10 +4529,10 @@
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G50" t="b">
         <v>1</v>
@@ -4558,10 +4561,10 @@
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G51" t="b">
         <v>1</v>
@@ -4590,16 +4593,16 @@
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G52" t="b">
         <v>1</v>
       </c>
       <c r="H52" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="I52">
         <v>1</v>
@@ -4622,10 +4625,10 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G53" t="b">
         <v>1</v>
@@ -4654,10 +4657,10 @@
         <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G54" t="b">
         <v>1</v>
@@ -4686,10 +4689,10 @@
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G55" t="b">
         <v>0</v>
@@ -4718,10 +4721,10 @@
         <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G56" t="b">
         <v>1</v>
@@ -4750,10 +4753,10 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G57" t="b">
         <v>1</v>
@@ -4782,10 +4785,10 @@
         <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G58" t="b">
         <v>1</v>
@@ -4814,16 +4817,16 @@
         <v>0</v>
       </c>
       <c r="E59" s="14" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="F59" s="16" t="s">
+        <v>785</v>
+      </c>
+      <c r="G59" t="b">
+        <v>1</v>
+      </c>
+      <c r="H59" s="14" t="s">
         <v>787</v>
-      </c>
-      <c r="G59" t="b">
-        <v>1</v>
-      </c>
-      <c r="H59" s="14" t="s">
-        <v>789</v>
       </c>
       <c r="I59">
         <v>1</v>
@@ -4846,10 +4849,10 @@
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="F60" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G60" t="b">
         <v>1</v>
@@ -5648,7 +5651,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="G27" t="b">
         <v>1</v>
@@ -5798,7 +5801,7 @@
         <v>1</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="I32">
         <v>1</v>
@@ -11154,14 +11157,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3C047F-07FE-4D94-87CE-EE299E4A7559}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B36" sqref="B35:B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11181,37 +11184,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>724</v>
+      </c>
+      <c r="B2" t="s">
+        <v>788</v>
+      </c>
+      <c r="C2" t="s">
+        <v>790</v>
+      </c>
+      <c r="D2" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>719</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D7" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>721</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D8" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>724</v>
-      </c>
-      <c r="C4" t="s">
-        <v>726</v>
-      </c>
-      <c r="D4" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>728</v>
+      </c>
+      <c r="D9" t="s">
         <v>729</v>
-      </c>
-      <c r="D5" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>